<commit_message>
Fix report-checklist secondo indicazioni
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GESTRIABXX/DM_RIABILITA/FSELink/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GESTRIABXX/DM_RIABILITA/FSELink/1.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrea\Documents\UILDM\Accreditamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E6A7F0-DB80-4B81-BA1F-3CC107797279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78AE37A-27AE-4B7D-9FC9-FCA03EAAD24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$193</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="480">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2318,7 +2318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2466,31 +2466,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{565105C8-FFD6-432C-8B2E-BD1D172FCD26}"/>
@@ -2793,7 +2768,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3938,14 +3913,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S31" sqref="S31"/>
+      <selection pane="bottomRight" activeCell="T129" sqref="T129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3959,7 +3933,8 @@
     <col min="8" max="8" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="18" width="36.42578125" customWidth="1"/>
+    <col min="11" max="11" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="36.42578125" customWidth="1"/>
     <col min="19" max="19" width="27.140625" customWidth="1"/>
     <col min="20" max="20" width="33.140625" customWidth="1"/>
     <col min="21" max="21" width="36.42578125" customWidth="1"/>
@@ -4234,7 +4209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -4273,7 +4248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>28</v>
       </c>
@@ -4312,7 +4287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -4351,7 +4326,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>30</v>
       </c>
@@ -4390,7 +4365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -4429,7 +4404,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -4452,7 +4427,9 @@
       <c r="J15" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="K15" s="38"/>
+      <c r="K15" s="38" t="s">
+        <v>234</v>
+      </c>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
@@ -4468,7 +4445,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>33</v>
       </c>
@@ -4507,7 +4484,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>34</v>
       </c>
@@ -4546,7 +4523,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>35</v>
       </c>
@@ -4585,7 +4562,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>36</v>
       </c>
@@ -4624,7 +4601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -4663,7 +4640,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>38</v>
       </c>
@@ -4702,7 +4679,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -4741,7 +4718,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -4764,7 +4741,9 @@
       <c r="J23" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="K23" s="38"/>
+      <c r="K23" s="38" t="s">
+        <v>234</v>
+      </c>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
@@ -4780,7 +4759,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>41</v>
       </c>
@@ -4819,7 +4798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>42</v>
       </c>
@@ -4858,7 +4837,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>43</v>
       </c>
@@ -4897,7 +4876,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="35">
         <v>44</v>
       </c>
@@ -4938,7 +4917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>45</v>
       </c>
@@ -4979,7 +4958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="35">
         <v>46</v>
       </c>
@@ -5020,7 +4999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -5086,7 +5065,9 @@
       </c>
       <c r="K31" s="38"/>
       <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
+      <c r="M31" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N31" s="38" t="s">
         <v>226</v>
       </c>
@@ -5112,7 +5093,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>49</v>
       </c>
@@ -5153,7 +5134,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>50</v>
       </c>
@@ -5194,7 +5175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>51</v>
       </c>
@@ -5235,7 +5216,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35">
         <v>53</v>
       </c>
@@ -5274,7 +5255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35">
         <v>55</v>
       </c>
@@ -5313,7 +5294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35">
         <v>56</v>
       </c>
@@ -5352,7 +5333,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="35">
         <v>57</v>
       </c>
@@ -5391,7 +5372,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35">
         <v>59</v>
       </c>
@@ -5430,7 +5411,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35">
         <v>60</v>
       </c>
@@ -5469,7 +5450,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35">
         <v>61</v>
       </c>
@@ -5508,7 +5489,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35">
         <v>62</v>
       </c>
@@ -5547,7 +5528,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35">
         <v>64</v>
       </c>
@@ -5586,7 +5567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>66</v>
       </c>
@@ -5625,7 +5606,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>67</v>
       </c>
@@ -5664,7 +5645,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>68</v>
       </c>
@@ -5703,7 +5684,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>69</v>
       </c>
@@ -5742,7 +5723,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35">
         <v>70</v>
       </c>
@@ -5781,7 +5762,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>71</v>
       </c>
@@ -5820,7 +5801,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>72</v>
       </c>
@@ -5859,7 +5840,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>73</v>
       </c>
@@ -5898,7 +5879,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>74</v>
       </c>
@@ -5937,7 +5918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="35">
         <v>76</v>
       </c>
@@ -5976,7 +5957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>78</v>
       </c>
@@ -6015,7 +5996,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="35">
         <v>79</v>
       </c>
@@ -6054,7 +6035,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>80</v>
       </c>
@@ -6093,7 +6074,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>81</v>
       </c>
@@ -6132,7 +6113,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>83</v>
       </c>
@@ -6171,7 +6152,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>84</v>
       </c>
@@ -6210,7 +6191,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>85</v>
       </c>
@@ -6249,7 +6230,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="35">
         <v>86</v>
       </c>
@@ -6288,7 +6269,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="35">
         <v>87</v>
       </c>
@@ -6327,7 +6308,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="35">
         <v>88</v>
       </c>
@@ -6366,7 +6347,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="35">
         <v>89</v>
       </c>
@@ -6405,7 +6386,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="35">
         <v>90</v>
       </c>
@@ -6444,7 +6425,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="35">
         <v>91</v>
       </c>
@@ -6483,7 +6464,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="35">
         <v>92</v>
       </c>
@@ -6522,7 +6503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="35">
         <v>93</v>
       </c>
@@ -6561,7 +6542,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="35">
         <v>95</v>
       </c>
@@ -6600,7 +6581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="35">
         <v>97</v>
       </c>
@@ -6639,7 +6620,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="35">
         <v>98</v>
       </c>
@@ -6678,7 +6659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="35">
         <v>99</v>
       </c>
@@ -6717,7 +6698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="35">
         <v>100</v>
       </c>
@@ -6756,7 +6737,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="35">
         <v>101</v>
       </c>
@@ -6795,7 +6776,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="35">
         <v>102</v>
       </c>
@@ -6834,7 +6815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="35">
         <v>103</v>
       </c>
@@ -6873,7 +6854,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="35">
         <v>104</v>
       </c>
@@ -6912,7 +6893,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="35">
         <v>105</v>
       </c>
@@ -6951,7 +6932,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="35">
         <v>106</v>
       </c>
@@ -6990,7 +6971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="35">
         <v>108</v>
       </c>
@@ -7029,7 +7010,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="35">
         <v>110</v>
       </c>
@@ -7068,7 +7049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="35">
         <v>111</v>
       </c>
@@ -7107,7 +7088,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="35">
         <v>112</v>
       </c>
@@ -7146,7 +7127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35">
         <v>113</v>
       </c>
@@ -7185,7 +7166,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="35">
         <v>114</v>
       </c>
@@ -7224,7 +7205,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="35">
         <v>115</v>
       </c>
@@ -7263,7 +7244,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="35">
         <v>116</v>
       </c>
@@ -7302,7 +7283,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="35">
         <v>117</v>
       </c>
@@ -7341,7 +7322,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="35">
         <v>118</v>
       </c>
@@ -7380,7 +7361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="35">
         <v>119</v>
       </c>
@@ -7419,7 +7400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="35">
         <v>120</v>
       </c>
@@ -7458,7 +7439,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="35">
         <v>121</v>
       </c>
@@ -7497,7 +7478,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="35">
         <v>123</v>
       </c>
@@ -7536,7 +7517,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="35">
         <v>125</v>
       </c>
@@ -7575,7 +7556,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="35">
         <v>126</v>
       </c>
@@ -7614,7 +7595,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35">
         <v>127</v>
       </c>
@@ -7653,7 +7634,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="35">
         <v>128</v>
       </c>
@@ -7692,7 +7673,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="35">
         <v>129</v>
       </c>
@@ -7731,7 +7712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="35">
         <v>130</v>
       </c>
@@ -7770,7 +7751,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="35">
         <v>131</v>
       </c>
@@ -7809,7 +7790,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="35">
         <v>132</v>
       </c>
@@ -7848,7 +7829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="35">
         <v>133</v>
       </c>
@@ -7887,7 +7868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <v>134</v>
       </c>
@@ -7926,7 +7907,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="35">
         <v>135</v>
       </c>
@@ -7965,7 +7946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="35">
         <v>136</v>
       </c>
@@ -8004,7 +7985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="35">
         <v>137</v>
       </c>
@@ -8043,7 +8024,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="35">
         <v>138</v>
       </c>
@@ -8082,7 +8063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35">
         <v>139</v>
       </c>
@@ -8121,7 +8102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>140</v>
       </c>
@@ -8160,7 +8141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="35">
         <v>141</v>
       </c>
@@ -8199,7 +8180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <v>142</v>
       </c>
@@ -8238,7 +8219,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="35">
         <v>143</v>
       </c>
@@ -8277,7 +8258,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="35">
         <v>144</v>
       </c>
@@ -8316,7 +8297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <v>145</v>
       </c>
@@ -8355,7 +8336,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="35">
         <v>146</v>
       </c>
@@ -8394,44 +8375,46 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" s="67" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="59">
+    <row r="116" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="35">
         <v>152</v>
       </c>
-      <c r="B116" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C116" s="60" t="s">
+      <c r="B116" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C116" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D116" s="59" t="s">
+      <c r="D116" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="E116" s="61" t="s">
+      <c r="E116" s="43" t="s">
         <v>329</v>
       </c>
-      <c r="F116" s="62">
+      <c r="F116" s="37">
         <v>46042</v>
       </c>
-      <c r="G116" s="62" t="s">
+      <c r="G116" s="37" t="s">
         <v>441</v>
       </c>
-      <c r="H116" s="62" t="s">
+      <c r="H116" s="37" t="s">
         <v>442</v>
       </c>
-      <c r="I116" s="63" t="s">
+      <c r="I116" s="42" t="s">
         <v>443</v>
       </c>
-      <c r="J116" s="64" t="s">
+      <c r="J116" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K116" s="64"/>
-      <c r="L116" s="64"/>
-      <c r="M116" s="64"/>
+      <c r="K116" s="38"/>
+      <c r="L116" s="38"/>
+      <c r="M116" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N116" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="O116" s="64"/>
+      <c r="O116" s="38"/>
       <c r="P116" s="38" t="s">
         <v>64</v>
       </c>
@@ -8444,51 +8427,53 @@
       <c r="S116" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="T116" s="64"/>
-      <c r="U116" s="65"/>
-      <c r="V116" s="66"/>
-      <c r="W116" s="64" t="s">
+      <c r="T116" s="38"/>
+      <c r="U116" s="39"/>
+      <c r="V116" s="40"/>
+      <c r="W116" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" s="67" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="59">
+    <row r="117" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="35">
         <v>154</v>
       </c>
-      <c r="B117" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C117" s="60" t="s">
+      <c r="B117" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C117" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D117" s="59" t="s">
+      <c r="D117" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="E117" s="61" t="s">
+      <c r="E117" s="43" t="s">
         <v>330</v>
       </c>
-      <c r="F117" s="62">
+      <c r="F117" s="37">
         <v>46042</v>
       </c>
-      <c r="G117" s="62" t="s">
+      <c r="G117" s="37" t="s">
         <v>444</v>
       </c>
-      <c r="H117" s="62" t="s">
+      <c r="H117" s="37" t="s">
         <v>442</v>
       </c>
-      <c r="I117" s="63" t="s">
+      <c r="I117" s="42" t="s">
         <v>445</v>
       </c>
-      <c r="J117" s="64" t="s">
+      <c r="J117" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K117" s="64"/>
-      <c r="L117" s="64"/>
-      <c r="M117" s="64"/>
+      <c r="K117" s="38"/>
+      <c r="L117" s="38"/>
+      <c r="M117" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N117" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="O117" s="64"/>
+      <c r="O117" s="38"/>
       <c r="P117" s="38" t="s">
         <v>64</v>
       </c>
@@ -8501,10 +8486,10 @@
       <c r="S117" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="T117" s="64"/>
-      <c r="U117" s="65"/>
-      <c r="V117" s="66"/>
-      <c r="W117" s="64" t="s">
+      <c r="T117" s="38"/>
+      <c r="U117" s="39"/>
+      <c r="V117" s="40"/>
+      <c r="W117" s="38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -8541,7 +8526,9 @@
       </c>
       <c r="K118" s="38"/>
       <c r="L118" s="38"/>
-      <c r="M118" s="38"/>
+      <c r="M118" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N118" s="38" t="s">
         <v>226</v>
       </c>
@@ -8598,7 +8585,9 @@
       </c>
       <c r="K119" s="38"/>
       <c r="L119" s="38"/>
-      <c r="M119" s="38"/>
+      <c r="M119" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N119" s="38" t="s">
         <v>226</v>
       </c>
@@ -8655,7 +8644,9 @@
       </c>
       <c r="K120" s="38"/>
       <c r="L120" s="38"/>
-      <c r="M120" s="38"/>
+      <c r="M120" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N120" s="38" t="s">
         <v>226</v>
       </c>
@@ -8712,7 +8703,9 @@
       </c>
       <c r="K121" s="38"/>
       <c r="L121" s="38"/>
-      <c r="M121" s="38"/>
+      <c r="M121" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N121" s="38" t="s">
         <v>226</v>
       </c>
@@ -8769,7 +8762,9 @@
       </c>
       <c r="K122" s="38"/>
       <c r="L122" s="38"/>
-      <c r="M122" s="38"/>
+      <c r="M122" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N122" s="38" t="s">
         <v>226</v>
       </c>
@@ -8826,7 +8821,9 @@
       </c>
       <c r="K123" s="38"/>
       <c r="L123" s="38"/>
-      <c r="M123" s="38"/>
+      <c r="M123" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N123" s="38" t="s">
         <v>226</v>
       </c>
@@ -8883,7 +8880,9 @@
       </c>
       <c r="K124" s="38"/>
       <c r="L124" s="38"/>
-      <c r="M124" s="38"/>
+      <c r="M124" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N124" s="38" t="s">
         <v>226</v>
       </c>
@@ -8940,7 +8939,9 @@
       </c>
       <c r="K125" s="38"/>
       <c r="L125" s="38"/>
-      <c r="M125" s="38"/>
+      <c r="M125" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N125" s="38" t="s">
         <v>226</v>
       </c>
@@ -8997,7 +8998,9 @@
       </c>
       <c r="K126" s="38"/>
       <c r="L126" s="38"/>
-      <c r="M126" s="38"/>
+      <c r="M126" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N126" s="38" t="s">
         <v>226</v>
       </c>
@@ -9054,7 +9057,9 @@
       </c>
       <c r="K127" s="38"/>
       <c r="L127" s="38"/>
-      <c r="M127" s="38"/>
+      <c r="M127" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N127" s="38" t="s">
         <v>226</v>
       </c>
@@ -9111,7 +9116,9 @@
       </c>
       <c r="K128" s="38"/>
       <c r="L128" s="38"/>
-      <c r="M128" s="38"/>
+      <c r="M128" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N128" s="38" t="s">
         <v>226</v>
       </c>
@@ -9168,7 +9175,9 @@
       </c>
       <c r="K129" s="38"/>
       <c r="L129" s="38"/>
-      <c r="M129" s="38"/>
+      <c r="M129" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N129" s="38" t="s">
         <v>226</v>
       </c>
@@ -9225,7 +9234,9 @@
       </c>
       <c r="K130" s="38"/>
       <c r="L130" s="38"/>
-      <c r="M130" s="38"/>
+      <c r="M130" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N130" s="38" t="s">
         <v>226</v>
       </c>
@@ -9249,7 +9260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="35">
         <v>175</v>
       </c>
@@ -9288,7 +9299,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="35">
         <v>177</v>
       </c>
@@ -9327,7 +9338,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="35">
         <v>178</v>
       </c>
@@ -9366,7 +9377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="35">
         <v>179</v>
       </c>
@@ -9405,7 +9416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="35">
         <v>180</v>
       </c>
@@ -9444,7 +9455,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="35">
         <v>181</v>
       </c>
@@ -9483,7 +9494,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="35">
         <v>182</v>
       </c>
@@ -9522,7 +9533,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="35">
         <v>183</v>
       </c>
@@ -9561,7 +9572,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="35">
         <v>184</v>
       </c>
@@ -9600,7 +9611,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="35">
         <v>185</v>
       </c>
@@ -9639,7 +9650,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="35">
         <v>186</v>
       </c>
@@ -9678,7 +9689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="35">
         <v>187</v>
       </c>
@@ -9717,7 +9728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="35">
         <v>188</v>
       </c>
@@ -9756,7 +9767,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="35">
         <v>189</v>
       </c>
@@ -9795,7 +9806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="35">
         <v>190</v>
       </c>
@@ -9834,7 +9845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="35">
         <v>191</v>
       </c>
@@ -9873,7 +9884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="35">
         <v>376</v>
       </c>
@@ -9912,7 +9923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="35">
         <v>417</v>
       </c>
@@ -9951,7 +9962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="35">
         <v>418</v>
       </c>
@@ -9990,7 +10001,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="35">
         <v>419</v>
       </c>
@@ -10029,7 +10040,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>423</v>
       </c>
@@ -10068,7 +10079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>424</v>
       </c>
@@ -10107,7 +10118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>425</v>
       </c>
@@ -10146,7 +10157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -10185,7 +10196,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -10224,7 +10235,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -10263,7 +10274,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -10302,7 +10313,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -10341,7 +10352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -10380,7 +10391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -10419,7 +10430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -10458,7 +10469,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -10497,7 +10508,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -10536,7 +10547,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="35">
         <v>448</v>
       </c>
@@ -10569,13 +10580,25 @@
       </c>
       <c r="K164" s="38"/>
       <c r="L164" s="38"/>
-      <c r="M164" s="38"/>
-      <c r="N164" s="38"/>
+      <c r="M164" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="N164" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="O164" s="38"/>
-      <c r="P164" s="38"/>
-      <c r="Q164" s="38"/>
-      <c r="R164" s="38"/>
-      <c r="S164" s="38"/>
+      <c r="P164" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q164" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="R164" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S164" s="38" t="s">
+        <v>479</v>
+      </c>
       <c r="T164" s="38"/>
       <c r="U164" s="39"/>
       <c r="V164" s="40"/>
@@ -10583,7 +10606,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="35">
         <v>449</v>
       </c>
@@ -10616,13 +10639,25 @@
       </c>
       <c r="K165" s="38"/>
       <c r="L165" s="38"/>
-      <c r="M165" s="38"/>
-      <c r="N165" s="38"/>
+      <c r="M165" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="N165" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="O165" s="38"/>
-      <c r="P165" s="38"/>
-      <c r="Q165" s="38"/>
-      <c r="R165" s="38"/>
-      <c r="S165" s="38"/>
+      <c r="P165" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q165" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="R165" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S165" s="38" t="s">
+        <v>479</v>
+      </c>
       <c r="T165" s="38"/>
       <c r="U165" s="39"/>
       <c r="V165" s="40"/>
@@ -10630,7 +10665,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="35">
         <v>450</v>
       </c>
@@ -10669,7 +10704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="35">
         <v>451</v>
       </c>
@@ -10708,7 +10743,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="35">
         <v>452</v>
       </c>
@@ -10747,7 +10782,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>454</v>
       </c>
@@ -10786,7 +10821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="35">
         <v>455</v>
       </c>
@@ -10825,7 +10860,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="35">
         <v>456</v>
       </c>
@@ -10864,7 +10899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="35">
         <v>457</v>
       </c>
@@ -10903,7 +10938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="35">
         <v>458</v>
       </c>
@@ -10942,7 +10977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="35">
         <v>459</v>
       </c>
@@ -10981,7 +11016,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="35">
         <v>460</v>
       </c>
@@ -11053,7 +11088,9 @@
       </c>
       <c r="K176" s="38"/>
       <c r="L176" s="35"/>
-      <c r="M176" s="38"/>
+      <c r="M176" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N176" s="38" t="s">
         <v>226</v>
       </c>
@@ -11077,7 +11114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="35">
         <v>462</v>
       </c>
@@ -11116,7 +11153,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="35">
         <v>463</v>
       </c>
@@ -11155,7 +11192,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="35">
         <v>464</v>
       </c>
@@ -11194,7 +11231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="35">
         <v>465</v>
       </c>
@@ -11233,7 +11270,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="35">
         <v>466</v>
       </c>
@@ -11272,7 +11309,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="35">
         <v>467</v>
       </c>
@@ -11344,7 +11381,9 @@
       </c>
       <c r="K183" s="38"/>
       <c r="L183" s="35"/>
-      <c r="M183" s="38"/>
+      <c r="M183" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N183" s="38" t="s">
         <v>226</v>
       </c>
@@ -11368,7 +11407,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="35">
         <v>469</v>
       </c>
@@ -11407,7 +11446,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="35">
         <v>470</v>
       </c>
@@ -11446,7 +11485,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="35">
         <v>471</v>
       </c>
@@ -11485,7 +11524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>472</v>
       </c>
@@ -11524,7 +11563,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="35">
         <v>473</v>
       </c>
@@ -11563,7 +11602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="35">
         <v>474</v>
       </c>
@@ -11635,7 +11674,9 @@
       </c>
       <c r="K190" s="38"/>
       <c r="L190" s="38"/>
-      <c r="M190" s="38"/>
+      <c r="M190" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="N190" s="38" t="s">
         <v>226</v>
       </c>
@@ -11659,7 +11700,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="35">
         <v>476</v>
       </c>
@@ -11698,7 +11739,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="35">
         <v>477</v>
       </c>
@@ -11737,7 +11778,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="35">
         <v>478</v>
       </c>
@@ -15733,18 +15774,7 @@
     <row r="749" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="750" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W193" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="22">
-      <filters>
-        <filter val="KO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:W193" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -18028,6 +18058,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -18171,22 +18216,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18204,31 +18259,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>